<commit_message>
Countinue code at denso(Update layout)
</commit_message>
<xml_diff>
--- a/Flow Received&Issues Goods.xlsx
+++ b/Flow Received&Issues Goods.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Stock Delivery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Stock Delivery\RIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C982E2CD-6283-46FA-A643-8A9A8E3D27FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88867B1A-9C13-4D12-8110-C161E234CBF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9540" windowHeight="7350" firstSheet="2" activeTab="5" xr2:uid="{83156955-99A9-4DAF-BEAE-AA98AB7D54E2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9540" windowHeight="7350" firstSheet="1" activeTab="1" xr2:uid="{83156955-99A9-4DAF-BEAE-AA98AB7D54E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow Xuất Kho" sheetId="1" r:id="rId1"/>
@@ -632,110 +632,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -761,6 +659,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -772,6 +679,99 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3488,15 +3488,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>926727</xdr:colOff>
+      <xdr:colOff>1702334</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>412741</xdr:rowOff>
+      <xdr:rowOff>358312</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1562598</xdr:colOff>
+      <xdr:colOff>2338205</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>653773</xdr:rowOff>
+      <xdr:rowOff>599344</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3511,7 +3511,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3156698" y="7035417"/>
+          <a:off x="3920298" y="9189348"/>
           <a:ext cx="635871" cy="241032"/>
         </a:xfrm>
         <a:prstGeom prst="can">
@@ -3655,15 +3655,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1244663</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>337766</xdr:rowOff>
+      <xdr:colOff>1636575</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2505653</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1245784</xdr:colOff>
+      <xdr:colOff>2020270</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>412741</xdr:rowOff>
+      <xdr:rowOff>358312</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3675,14 +3675,14 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="255" idx="3"/>
+          <a:stCxn id="56" idx="2"/>
           <a:endCxn id="49" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="3474634" y="6557031"/>
-          <a:ext cx="1121" cy="478386"/>
+        <a:xfrm>
+          <a:off x="3854539" y="7390617"/>
+          <a:ext cx="383695" cy="1798731"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4177,15 +4177,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1052791</xdr:colOff>
+      <xdr:colOff>1828398</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>221319</xdr:rowOff>
+      <xdr:rowOff>248534</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1444997</xdr:colOff>
+      <xdr:colOff>2220604</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>570187</xdr:rowOff>
+      <xdr:rowOff>597402</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4208,7 +4208,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3282762" y="7538760"/>
+          <a:off x="4046362" y="9773534"/>
           <a:ext cx="392206" cy="348868"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5491,13 +5491,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>523231</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>395753</xdr:rowOff>
+      <xdr:rowOff>409423</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1052791</xdr:colOff>
+      <xdr:colOff>1828398</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>409423</xdr:rowOff>
+      <xdr:rowOff>422968</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5514,9 +5514,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="2753202" y="7713194"/>
-          <a:ext cx="529560" cy="13670"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2741195" y="9934423"/>
+          <a:ext cx="1305167" cy="13545"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5545,15 +5545,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1244663</xdr:colOff>
+      <xdr:colOff>2020270</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>653773</xdr:rowOff>
+      <xdr:rowOff>599344</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1248894</xdr:colOff>
+      <xdr:colOff>2024501</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>221319</xdr:rowOff>
+      <xdr:rowOff>248534</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5571,8 +5571,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3474634" y="7276449"/>
-          <a:ext cx="4231" cy="262311"/>
+          <a:off x="4238234" y="9430380"/>
+          <a:ext cx="4231" cy="343154"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -12537,8 +12537,8 @@
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>58144</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>-1</xdr:rowOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17114,8 +17114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1E23DA-7F5F-464F-97DA-E9107727AA6D}">
   <dimension ref="B1:W113"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -18221,52 +18221,52 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="104" t="s">
+      <c r="C2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
-      <c r="N2" s="105"/>
-      <c r="O2" s="105"/>
-      <c r="P2" s="105"/>
-      <c r="Q2" s="105"/>
-      <c r="R2" s="105"/>
-      <c r="S2" s="105"/>
-      <c r="T2" s="106"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="72"/>
     </row>
     <row r="3" spans="2:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="69"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="75"/>
       <c r="F3" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="67" t="s">
+      <c r="G3" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="68"/>
-      <c r="I3" s="69"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="75"/>
       <c r="J3" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="67" t="s">
+      <c r="K3" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="68"/>
-      <c r="M3" s="69"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="75"/>
       <c r="N3" s="32"/>
       <c r="O3" s="32"/>
       <c r="P3" s="32"/>
@@ -18279,58 +18279,58 @@
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="99"/>
-      <c r="E4" s="100"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="66"/>
       <c r="F4" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="73" t="s">
+      <c r="G4" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
       <c r="J4" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="107" t="s">
+      <c r="K4" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="107"/>
-      <c r="M4" s="107"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="108"/>
-      <c r="P4" s="108"/>
-      <c r="Q4" s="108"/>
-      <c r="R4" s="109"/>
-      <c r="S4" s="108"/>
-      <c r="T4" s="110"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="78"/>
+      <c r="S4" s="77"/>
+      <c r="T4" s="79"/>
     </row>
     <row r="5" spans="2:23" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="99"/>
-      <c r="E5" s="100"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="66"/>
       <c r="F5" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="99"/>
-      <c r="I5" s="100"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="66"/>
       <c r="J5" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="101"/>
-      <c r="L5" s="102"/>
-      <c r="M5" s="103"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="69"/>
       <c r="N5" s="63"/>
       <c r="O5" s="39"/>
       <c r="P5" s="39"/>
@@ -18343,116 +18343,116 @@
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="92"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="94"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="82"/>
       <c r="F6"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="95"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="85"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="98" t="s">
+      <c r="K6" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="L6" s="98"/>
-      <c r="M6" s="98"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
       <c r="N6" s="4"/>
-      <c r="O6" s="96"/>
-      <c r="P6" s="96"/>
-      <c r="Q6" s="96"/>
-      <c r="R6" s="96"/>
-      <c r="S6" s="96"/>
-      <c r="T6" s="97"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="87"/>
+      <c r="T6" s="88"/>
     </row>
     <row r="7" spans="2:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="92"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="94"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="82"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="95"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="85"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="96"/>
-      <c r="L7" s="96"/>
-      <c r="M7" s="96"/>
+      <c r="K7" s="87"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
       <c r="N7" s="7"/>
-      <c r="O7" s="96"/>
-      <c r="P7" s="96"/>
-      <c r="Q7" s="96"/>
-      <c r="R7" s="96"/>
-      <c r="S7" s="96"/>
-      <c r="T7" s="97"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
+      <c r="S7" s="87"/>
+      <c r="T7" s="88"/>
     </row>
     <row r="8" spans="2:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="92"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="94"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="82"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="95"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="85"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
-      <c r="M8" s="96"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="87"/>
       <c r="N8" s="7"/>
-      <c r="O8" s="96"/>
-      <c r="P8" s="96"/>
-      <c r="Q8" s="96"/>
-      <c r="R8" s="96"/>
-      <c r="S8" s="96"/>
-      <c r="T8" s="97"/>
+      <c r="O8" s="87"/>
+      <c r="P8" s="87"/>
+      <c r="Q8" s="87"/>
+      <c r="R8" s="87"/>
+      <c r="S8" s="87"/>
+      <c r="T8" s="88"/>
     </row>
     <row r="9" spans="2:23" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="92"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="94"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="82"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="95"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="85"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="96"/>
-      <c r="L9" s="96"/>
-      <c r="M9" s="96"/>
+      <c r="K9" s="87"/>
+      <c r="L9" s="87"/>
+      <c r="M9" s="87"/>
       <c r="N9" s="7"/>
-      <c r="O9" s="96"/>
-      <c r="P9" s="96"/>
-      <c r="Q9" s="96"/>
-      <c r="R9" s="96"/>
-      <c r="S9" s="96"/>
-      <c r="T9" s="97"/>
+      <c r="O9" s="87"/>
+      <c r="P9" s="87"/>
+      <c r="Q9" s="87"/>
+      <c r="R9" s="87"/>
+      <c r="S9" s="87"/>
+      <c r="T9" s="88"/>
     </row>
     <row r="10" spans="2:23" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="93"/>
-      <c r="E10" s="94"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="82"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="95"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="85"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="96"/>
-      <c r="L10" s="96"/>
-      <c r="M10" s="96"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="87"/>
+      <c r="M10" s="87"/>
       <c r="N10" s="4"/>
-      <c r="O10" s="96"/>
-      <c r="P10" s="96"/>
-      <c r="Q10" s="96"/>
-      <c r="R10" s="96"/>
-      <c r="S10" s="96"/>
-      <c r="T10" s="97"/>
+      <c r="O10" s="87"/>
+      <c r="P10" s="87"/>
+      <c r="Q10" s="87"/>
+      <c r="R10" s="87"/>
+      <c r="S10" s="87"/>
+      <c r="T10" s="88"/>
     </row>
     <row r="11" spans="2:23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
@@ -18471,25 +18471,25 @@
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="12"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="78"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="91"/>
       <c r="J12" s="13"/>
-      <c r="K12" s="76"/>
-      <c r="L12" s="77"/>
-      <c r="M12" s="78"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="90"/>
+      <c r="M12" s="91"/>
       <c r="N12" s="13"/>
-      <c r="O12" s="76"/>
-      <c r="P12" s="77"/>
-      <c r="Q12" s="78"/>
-      <c r="R12" s="88"/>
-      <c r="S12" s="88"/>
-      <c r="T12" s="89"/>
-      <c r="U12" s="76" t="s">
+      <c r="O12" s="89"/>
+      <c r="P12" s="90"/>
+      <c r="Q12" s="91"/>
+      <c r="R12" s="92"/>
+      <c r="S12" s="92"/>
+      <c r="T12" s="93"/>
+      <c r="U12" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="V12" s="77"/>
-      <c r="W12" s="78"/>
+      <c r="V12" s="90"/>
+      <c r="W12" s="91"/>
     </row>
     <row r="13" spans="2:23" s="24" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -18503,21 +18503,21 @@
       <c r="H13" s="17"/>
       <c r="I13" s="18"/>
       <c r="J13" s="17"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="80"/>
-      <c r="M13" s="80"/>
-      <c r="N13" s="80"/>
-      <c r="O13" s="80"/>
-      <c r="P13" s="80"/>
-      <c r="Q13" s="81"/>
-      <c r="R13" s="90"/>
-      <c r="S13" s="90"/>
-      <c r="T13" s="91"/>
-      <c r="U13" s="79" t="s">
+      <c r="K13" s="94"/>
+      <c r="L13" s="95"/>
+      <c r="M13" s="95"/>
+      <c r="N13" s="95"/>
+      <c r="O13" s="95"/>
+      <c r="P13" s="95"/>
+      <c r="Q13" s="96"/>
+      <c r="R13" s="97"/>
+      <c r="S13" s="97"/>
+      <c r="T13" s="98"/>
+      <c r="U13" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="V13" s="80"/>
-      <c r="W13" s="81"/>
+      <c r="V13" s="95"/>
+      <c r="W13" s="96"/>
     </row>
     <row r="14" spans="2:23" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
@@ -18527,25 +18527,25 @@
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="66"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="84"/>
+      <c r="I14" s="99"/>
       <c r="J14" s="20"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="66"/>
+      <c r="K14" s="83"/>
+      <c r="L14" s="84"/>
+      <c r="M14" s="99"/>
       <c r="N14" s="20"/>
-      <c r="O14" s="64"/>
-      <c r="P14" s="65"/>
-      <c r="Q14" s="66"/>
-      <c r="R14" s="64"/>
-      <c r="S14" s="65"/>
-      <c r="T14" s="66"/>
-      <c r="U14" s="64" t="s">
+      <c r="O14" s="83"/>
+      <c r="P14" s="84"/>
+      <c r="Q14" s="99"/>
+      <c r="R14" s="83"/>
+      <c r="S14" s="84"/>
+      <c r="T14" s="99"/>
+      <c r="U14" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="V14" s="65"/>
-      <c r="W14" s="66"/>
+      <c r="V14" s="84"/>
+      <c r="W14" s="99"/>
     </row>
     <row r="15" spans="2:23" s="23" customFormat="1" ht="55.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
@@ -18555,25 +18555,25 @@
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="84"/>
+      <c r="G15" s="100"/>
+      <c r="H15" s="101"/>
+      <c r="I15" s="102"/>
       <c r="J15" s="21"/>
-      <c r="K15" s="82"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="84"/>
+      <c r="K15" s="100"/>
+      <c r="L15" s="101"/>
+      <c r="M15" s="102"/>
       <c r="N15" s="21"/>
-      <c r="O15" s="82"/>
-      <c r="P15" s="83"/>
-      <c r="Q15" s="84"/>
-      <c r="R15" s="82"/>
-      <c r="S15" s="83"/>
-      <c r="T15" s="84"/>
-      <c r="U15" s="82" t="s">
+      <c r="O15" s="100"/>
+      <c r="P15" s="101"/>
+      <c r="Q15" s="102"/>
+      <c r="R15" s="100"/>
+      <c r="S15" s="101"/>
+      <c r="T15" s="102"/>
+      <c r="U15" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="V15" s="83"/>
-      <c r="W15" s="84"/>
+      <c r="V15" s="101"/>
+      <c r="W15" s="102"/>
     </row>
     <row r="16" spans="2:23" ht="93.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
@@ -18583,23 +18583,23 @@
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="66"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="99"/>
       <c r="J16" s="20"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="65"/>
-      <c r="M16" s="66"/>
+      <c r="K16" s="83"/>
+      <c r="L16" s="84"/>
+      <c r="M16" s="99"/>
       <c r="N16" s="20"/>
-      <c r="O16" s="64"/>
-      <c r="P16" s="65"/>
-      <c r="Q16" s="66"/>
-      <c r="R16" s="64"/>
-      <c r="S16" s="65"/>
-      <c r="T16" s="66"/>
-      <c r="U16" s="64"/>
-      <c r="V16" s="65"/>
-      <c r="W16" s="66"/>
+      <c r="O16" s="83"/>
+      <c r="P16" s="84"/>
+      <c r="Q16" s="99"/>
+      <c r="R16" s="83"/>
+      <c r="S16" s="84"/>
+      <c r="T16" s="99"/>
+      <c r="U16" s="83"/>
+      <c r="V16" s="84"/>
+      <c r="W16" s="99"/>
     </row>
     <row r="17" spans="2:23" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
@@ -18609,23 +18609,23 @@
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="66"/>
+      <c r="G17" s="83"/>
+      <c r="H17" s="84"/>
+      <c r="I17" s="99"/>
       <c r="J17" s="20"/>
-      <c r="K17" s="64"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="66"/>
+      <c r="K17" s="83"/>
+      <c r="L17" s="84"/>
+      <c r="M17" s="99"/>
       <c r="N17" s="20"/>
-      <c r="O17" s="64"/>
-      <c r="P17" s="65"/>
-      <c r="Q17" s="66"/>
-      <c r="R17" s="64"/>
-      <c r="S17" s="65"/>
-      <c r="T17" s="66"/>
-      <c r="U17" s="64"/>
-      <c r="V17" s="65"/>
-      <c r="W17" s="66"/>
+      <c r="O17" s="83"/>
+      <c r="P17" s="84"/>
+      <c r="Q17" s="99"/>
+      <c r="R17" s="83"/>
+      <c r="S17" s="84"/>
+      <c r="T17" s="99"/>
+      <c r="U17" s="83"/>
+      <c r="V17" s="84"/>
+      <c r="W17" s="99"/>
     </row>
     <row r="18" spans="2:23" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
@@ -18635,23 +18635,23 @@
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="85"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="87"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="104"/>
+      <c r="I18" s="105"/>
       <c r="J18" s="22"/>
-      <c r="K18" s="85"/>
-      <c r="L18" s="86"/>
-      <c r="M18" s="87"/>
+      <c r="K18" s="103"/>
+      <c r="L18" s="104"/>
+      <c r="M18" s="105"/>
       <c r="N18" s="22"/>
-      <c r="O18" s="85"/>
-      <c r="P18" s="86"/>
-      <c r="Q18" s="87"/>
-      <c r="R18" s="64"/>
-      <c r="S18" s="65"/>
-      <c r="T18" s="66"/>
-      <c r="U18" s="64"/>
-      <c r="V18" s="65"/>
-      <c r="W18" s="66"/>
+      <c r="O18" s="103"/>
+      <c r="P18" s="104"/>
+      <c r="Q18" s="105"/>
+      <c r="R18" s="83"/>
+      <c r="S18" s="84"/>
+      <c r="T18" s="99"/>
+      <c r="U18" s="83"/>
+      <c r="V18" s="84"/>
+      <c r="W18" s="99"/>
     </row>
     <row r="19" spans="2:23" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R19" s="23"/>
@@ -18678,17 +18678,17 @@
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="12"/>
-      <c r="G21" s="76"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="78"/>
+      <c r="G21" s="89"/>
+      <c r="H21" s="90"/>
+      <c r="I21" s="91"/>
       <c r="J21" s="13"/>
-      <c r="K21" s="76"/>
-      <c r="L21" s="77"/>
-      <c r="M21" s="78"/>
+      <c r="K21" s="89"/>
+      <c r="L21" s="90"/>
+      <c r="M21" s="91"/>
       <c r="N21" s="13"/>
-      <c r="O21" s="76"/>
-      <c r="P21" s="77"/>
-      <c r="Q21" s="78"/>
+      <c r="O21" s="89"/>
+      <c r="P21" s="90"/>
+      <c r="Q21" s="91"/>
     </row>
     <row r="22" spans="2:23" s="24" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
@@ -18702,13 +18702,13 @@
       <c r="H22" s="17"/>
       <c r="I22" s="18"/>
       <c r="J22" s="17"/>
-      <c r="K22" s="79"/>
-      <c r="L22" s="80"/>
-      <c r="M22" s="80"/>
-      <c r="N22" s="80"/>
-      <c r="O22" s="80"/>
-      <c r="P22" s="80"/>
-      <c r="Q22" s="81"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="95"/>
+      <c r="M22" s="95"/>
+      <c r="N22" s="95"/>
+      <c r="O22" s="95"/>
+      <c r="P22" s="95"/>
+      <c r="Q22" s="96"/>
     </row>
     <row r="23" spans="2:23" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
@@ -18718,17 +18718,17 @@
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="66"/>
+      <c r="G23" s="83"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="99"/>
       <c r="J23" s="20"/>
-      <c r="K23" s="64"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="66"/>
+      <c r="K23" s="83"/>
+      <c r="L23" s="84"/>
+      <c r="M23" s="99"/>
       <c r="N23" s="20"/>
-      <c r="O23" s="64"/>
-      <c r="P23" s="65"/>
-      <c r="Q23" s="66"/>
+      <c r="O23" s="83"/>
+      <c r="P23" s="84"/>
+      <c r="Q23" s="99"/>
     </row>
     <row r="24" spans="2:23" s="23" customFormat="1" ht="55.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
@@ -18738,17 +18738,17 @@
       <c r="D24" s="19"/>
       <c r="E24" s="19"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="82"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="84"/>
+      <c r="G24" s="100"/>
+      <c r="H24" s="101"/>
+      <c r="I24" s="102"/>
       <c r="J24" s="21"/>
-      <c r="K24" s="82"/>
-      <c r="L24" s="83"/>
-      <c r="M24" s="84"/>
+      <c r="K24" s="100"/>
+      <c r="L24" s="101"/>
+      <c r="M24" s="102"/>
       <c r="N24" s="21"/>
-      <c r="O24" s="82"/>
-      <c r="P24" s="83"/>
-      <c r="Q24" s="84"/>
+      <c r="O24" s="100"/>
+      <c r="P24" s="101"/>
+      <c r="Q24" s="102"/>
     </row>
     <row r="25" spans="2:23" ht="99.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
@@ -18758,17 +18758,17 @@
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="66"/>
+      <c r="G25" s="83"/>
+      <c r="H25" s="84"/>
+      <c r="I25" s="99"/>
       <c r="J25" s="20"/>
-      <c r="K25" s="64"/>
-      <c r="L25" s="65"/>
-      <c r="M25" s="66"/>
+      <c r="K25" s="83"/>
+      <c r="L25" s="84"/>
+      <c r="M25" s="99"/>
       <c r="N25" s="20"/>
-      <c r="O25" s="64"/>
-      <c r="P25" s="65"/>
-      <c r="Q25" s="66"/>
+      <c r="O25" s="83"/>
+      <c r="P25" s="84"/>
+      <c r="Q25" s="99"/>
     </row>
     <row r="26" spans="2:23" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
@@ -18778,17 +18778,17 @@
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="85"/>
-      <c r="H26" s="86"/>
-      <c r="I26" s="87"/>
+      <c r="G26" s="103"/>
+      <c r="H26" s="104"/>
+      <c r="I26" s="105"/>
       <c r="J26" s="22"/>
-      <c r="K26" s="85"/>
-      <c r="L26" s="86"/>
-      <c r="M26" s="87"/>
+      <c r="K26" s="103"/>
+      <c r="L26" s="104"/>
+      <c r="M26" s="105"/>
       <c r="N26" s="22"/>
-      <c r="O26" s="85"/>
-      <c r="P26" s="86"/>
-      <c r="Q26" s="87"/>
+      <c r="O26" s="103"/>
+      <c r="P26" s="104"/>
+      <c r="Q26" s="105"/>
     </row>
     <row r="27" spans="2:23" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="2:23" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18800,26 +18800,26 @@
     </row>
     <row r="33" spans="2:20" s="29" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="25"/>
-      <c r="C33" s="70"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="72"/>
+      <c r="C33" s="106"/>
+      <c r="D33" s="107"/>
+      <c r="E33" s="108"/>
       <c r="F33" s="26"/>
-      <c r="G33" s="70" t="s">
+      <c r="G33" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="H33" s="71"/>
-      <c r="I33" s="72"/>
+      <c r="H33" s="107"/>
+      <c r="I33" s="108"/>
       <c r="J33" s="27"/>
-      <c r="K33" s="73"/>
-      <c r="L33" s="71"/>
-      <c r="M33" s="72"/>
+      <c r="K33" s="64"/>
+      <c r="L33" s="107"/>
+      <c r="M33" s="108"/>
       <c r="N33" s="27"/>
-      <c r="O33" s="73"/>
-      <c r="P33" s="74"/>
-      <c r="Q33" s="75"/>
-      <c r="R33" s="70"/>
-      <c r="S33" s="71"/>
-      <c r="T33" s="72"/>
+      <c r="O33" s="64"/>
+      <c r="P33" s="109"/>
+      <c r="Q33" s="110"/>
+      <c r="R33" s="106"/>
+      <c r="S33" s="107"/>
+      <c r="T33" s="108"/>
     </row>
     <row r="34" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="2:20" ht="18" x14ac:dyDescent="0.25">
@@ -18836,81 +18836,6 @@
     </row>
   </sheetData>
   <mergeCells count="91">
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="C2:T2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="R12:T12"/>
-    <mergeCell ref="K13:Q13"/>
-    <mergeCell ref="R13:T13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="O14:Q14"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="O15:Q15"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="O16:Q16"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="O17:Q17"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="O21:Q21"/>
-    <mergeCell ref="O25:Q25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="O26:Q26"/>
-    <mergeCell ref="K22:Q22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="O23:Q23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="O24:Q24"/>
     <mergeCell ref="U17:W17"/>
     <mergeCell ref="U18:W18"/>
     <mergeCell ref="G3:I3"/>
@@ -18927,6 +18852,81 @@
     <mergeCell ref="U16:W16"/>
     <mergeCell ref="G25:I25"/>
     <mergeCell ref="K25:M25"/>
+    <mergeCell ref="O25:Q25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="O26:Q26"/>
+    <mergeCell ref="K22:Q22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="O23:Q23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="O24:Q24"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="O21:Q21"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="O14:Q14"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="R12:T12"/>
+    <mergeCell ref="K13:Q13"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="C2:T2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="C5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -18969,7 +18969,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U49" sqref="U49"/>
+      <selection activeCell="V62" sqref="V62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18983,7 +18983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7723D05E-F6B5-4206-A197-FBC6170C66D3}">
   <dimension ref="B1:W112"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -20090,48 +20090,48 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="104" t="s">
+      <c r="C2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
-      <c r="N2" s="105"/>
-      <c r="O2" s="105"/>
-      <c r="P2" s="105"/>
-      <c r="Q2" s="105"/>
-      <c r="R2" s="105"/>
-      <c r="S2" s="105"/>
-      <c r="T2" s="106"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="72"/>
     </row>
     <row r="3" spans="2:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="69"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="75"/>
       <c r="F3" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="67" t="s">
+      <c r="G3" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="68"/>
-      <c r="I3" s="69"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="75"/>
       <c r="J3" s="36"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="69"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="75"/>
       <c r="N3" s="32"/>
       <c r="O3" s="32"/>
       <c r="P3" s="32"/>
@@ -20144,52 +20144,52 @@
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="99"/>
-      <c r="E4" s="100"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="66"/>
       <c r="F4" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="73" t="s">
+      <c r="G4" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
       <c r="J4" s="58"/>
-      <c r="K4" s="107" t="s">
+      <c r="K4" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="107"/>
-      <c r="M4" s="107"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="108"/>
-      <c r="P4" s="108"/>
-      <c r="Q4" s="108"/>
-      <c r="R4" s="109"/>
-      <c r="S4" s="108"/>
-      <c r="T4" s="110"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="78"/>
+      <c r="S4" s="77"/>
+      <c r="T4" s="79"/>
     </row>
     <row r="5" spans="2:23" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="99"/>
-      <c r="E5" s="100"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="66"/>
       <c r="F5" s="62"/>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="99"/>
-      <c r="I5" s="100"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="66"/>
       <c r="J5" s="45"/>
-      <c r="K5" s="101"/>
-      <c r="L5" s="102"/>
-      <c r="M5" s="103"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="69"/>
       <c r="N5" s="63"/>
       <c r="O5" s="59"/>
       <c r="P5" s="59"/>
@@ -20202,93 +20202,93 @@
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="92"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="94"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="82"/>
       <c r="F6"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="95"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="85"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="98" t="s">
+      <c r="K6" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="L6" s="98"/>
-      <c r="M6" s="98"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
       <c r="N6" s="4"/>
-      <c r="O6" s="96"/>
-      <c r="P6" s="96"/>
-      <c r="Q6" s="96"/>
-      <c r="R6" s="96"/>
-      <c r="S6" s="96"/>
-      <c r="T6" s="97"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="87"/>
+      <c r="T6" s="88"/>
     </row>
     <row r="7" spans="2:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="92"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="94"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="82"/>
       <c r="F7" s="53"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="95"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="85"/>
       <c r="J7" s="54"/>
-      <c r="K7" s="96"/>
-      <c r="L7" s="96"/>
-      <c r="M7" s="96"/>
+      <c r="K7" s="87"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
       <c r="N7" s="55"/>
-      <c r="O7" s="96"/>
-      <c r="P7" s="96"/>
-      <c r="Q7" s="96"/>
-      <c r="R7" s="96"/>
-      <c r="S7" s="96"/>
-      <c r="T7" s="97"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
+      <c r="S7" s="87"/>
+      <c r="T7" s="88"/>
     </row>
     <row r="8" spans="2:23" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="92"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="94"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="82"/>
       <c r="F8" s="53"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="95"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="85"/>
       <c r="J8" s="54"/>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
-      <c r="M8" s="96"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="87"/>
       <c r="N8" s="55"/>
-      <c r="O8" s="96"/>
-      <c r="P8" s="96"/>
-      <c r="Q8" s="96"/>
-      <c r="R8" s="96"/>
-      <c r="S8" s="96"/>
-      <c r="T8" s="97"/>
+      <c r="O8" s="87"/>
+      <c r="P8" s="87"/>
+      <c r="Q8" s="87"/>
+      <c r="R8" s="87"/>
+      <c r="S8" s="87"/>
+      <c r="T8" s="88"/>
     </row>
     <row r="9" spans="2:23" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="94"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="82"/>
       <c r="F9" s="53"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="95"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="85"/>
       <c r="J9" s="54"/>
-      <c r="K9" s="96"/>
-      <c r="L9" s="96"/>
-      <c r="M9" s="96"/>
+      <c r="K9" s="87"/>
+      <c r="L9" s="87"/>
+      <c r="M9" s="87"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="96"/>
-      <c r="P9" s="96"/>
-      <c r="Q9" s="96"/>
-      <c r="R9" s="96"/>
-      <c r="S9" s="96"/>
-      <c r="T9" s="97"/>
+      <c r="O9" s="87"/>
+      <c r="P9" s="87"/>
+      <c r="Q9" s="87"/>
+      <c r="R9" s="87"/>
+      <c r="S9" s="87"/>
+      <c r="T9" s="88"/>
     </row>
     <row r="10" spans="2:23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
@@ -20307,25 +20307,25 @@
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="12"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="78"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="91"/>
       <c r="J11" s="46"/>
-      <c r="K11" s="76"/>
-      <c r="L11" s="77"/>
-      <c r="M11" s="78"/>
+      <c r="K11" s="89"/>
+      <c r="L11" s="90"/>
+      <c r="M11" s="91"/>
       <c r="N11" s="46"/>
-      <c r="O11" s="76"/>
-      <c r="P11" s="77"/>
-      <c r="Q11" s="78"/>
-      <c r="R11" s="88"/>
-      <c r="S11" s="88"/>
-      <c r="T11" s="89"/>
-      <c r="U11" s="76" t="s">
+      <c r="O11" s="89"/>
+      <c r="P11" s="90"/>
+      <c r="Q11" s="91"/>
+      <c r="R11" s="92"/>
+      <c r="S11" s="92"/>
+      <c r="T11" s="93"/>
+      <c r="U11" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="V11" s="77"/>
-      <c r="W11" s="78"/>
+      <c r="V11" s="90"/>
+      <c r="W11" s="91"/>
     </row>
     <row r="12" spans="2:23" s="24" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -20339,21 +20339,21 @@
       <c r="H12" s="48"/>
       <c r="I12" s="49"/>
       <c r="J12" s="48"/>
-      <c r="K12" s="79"/>
-      <c r="L12" s="80"/>
-      <c r="M12" s="80"/>
-      <c r="N12" s="80"/>
-      <c r="O12" s="80"/>
-      <c r="P12" s="80"/>
-      <c r="Q12" s="81"/>
-      <c r="R12" s="90"/>
-      <c r="S12" s="90"/>
-      <c r="T12" s="91"/>
-      <c r="U12" s="79" t="s">
+      <c r="K12" s="94"/>
+      <c r="L12" s="95"/>
+      <c r="M12" s="95"/>
+      <c r="N12" s="95"/>
+      <c r="O12" s="95"/>
+      <c r="P12" s="95"/>
+      <c r="Q12" s="96"/>
+      <c r="R12" s="97"/>
+      <c r="S12" s="97"/>
+      <c r="T12" s="98"/>
+      <c r="U12" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="V12" s="80"/>
-      <c r="W12" s="81"/>
+      <c r="V12" s="95"/>
+      <c r="W12" s="96"/>
     </row>
     <row r="13" spans="2:23" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
@@ -20363,25 +20363,25 @@
       <c r="D13" s="52"/>
       <c r="E13" s="52"/>
       <c r="F13" s="53"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="66"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="84"/>
+      <c r="I13" s="99"/>
       <c r="J13" s="42"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="65"/>
-      <c r="M13" s="66"/>
+      <c r="K13" s="83"/>
+      <c r="L13" s="84"/>
+      <c r="M13" s="99"/>
       <c r="N13" s="42"/>
-      <c r="O13" s="64"/>
-      <c r="P13" s="65"/>
-      <c r="Q13" s="66"/>
-      <c r="R13" s="64"/>
-      <c r="S13" s="65"/>
-      <c r="T13" s="66"/>
-      <c r="U13" s="64" t="s">
+      <c r="O13" s="83"/>
+      <c r="P13" s="84"/>
+      <c r="Q13" s="99"/>
+      <c r="R13" s="83"/>
+      <c r="S13" s="84"/>
+      <c r="T13" s="99"/>
+      <c r="U13" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="V13" s="65"/>
-      <c r="W13" s="66"/>
+      <c r="V13" s="84"/>
+      <c r="W13" s="99"/>
     </row>
     <row r="14" spans="2:23" s="23" customFormat="1" ht="55.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
@@ -20391,25 +20391,25 @@
       <c r="D14" s="52"/>
       <c r="E14" s="52"/>
       <c r="F14" s="53"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="84"/>
+      <c r="G14" s="100"/>
+      <c r="H14" s="101"/>
+      <c r="I14" s="102"/>
       <c r="J14" s="50"/>
-      <c r="K14" s="82"/>
-      <c r="L14" s="83"/>
-      <c r="M14" s="84"/>
+      <c r="K14" s="100"/>
+      <c r="L14" s="101"/>
+      <c r="M14" s="102"/>
       <c r="N14" s="50"/>
-      <c r="O14" s="82"/>
-      <c r="P14" s="83"/>
-      <c r="Q14" s="84"/>
-      <c r="R14" s="82"/>
-      <c r="S14" s="83"/>
-      <c r="T14" s="84"/>
-      <c r="U14" s="82" t="s">
+      <c r="O14" s="100"/>
+      <c r="P14" s="101"/>
+      <c r="Q14" s="102"/>
+      <c r="R14" s="100"/>
+      <c r="S14" s="101"/>
+      <c r="T14" s="102"/>
+      <c r="U14" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="V14" s="83"/>
-      <c r="W14" s="84"/>
+      <c r="V14" s="101"/>
+      <c r="W14" s="102"/>
     </row>
     <row r="15" spans="2:23" ht="93.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
@@ -20419,23 +20419,23 @@
       <c r="D15" s="52"/>
       <c r="E15" s="52"/>
       <c r="F15" s="53"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="66"/>
+      <c r="G15" s="83"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="99"/>
       <c r="J15" s="42"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="66"/>
+      <c r="K15" s="83"/>
+      <c r="L15" s="84"/>
+      <c r="M15" s="99"/>
       <c r="N15" s="42"/>
-      <c r="O15" s="64"/>
-      <c r="P15" s="65"/>
-      <c r="Q15" s="66"/>
-      <c r="R15" s="64"/>
-      <c r="S15" s="65"/>
-      <c r="T15" s="66"/>
-      <c r="U15" s="64"/>
-      <c r="V15" s="65"/>
-      <c r="W15" s="66"/>
+      <c r="O15" s="83"/>
+      <c r="P15" s="84"/>
+      <c r="Q15" s="99"/>
+      <c r="R15" s="83"/>
+      <c r="S15" s="84"/>
+      <c r="T15" s="99"/>
+      <c r="U15" s="83"/>
+      <c r="V15" s="84"/>
+      <c r="W15" s="99"/>
     </row>
     <row r="16" spans="2:23" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
@@ -20445,23 +20445,23 @@
       <c r="D16" s="52"/>
       <c r="E16" s="52"/>
       <c r="F16" s="53"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="66"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="99"/>
       <c r="J16" s="42"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="65"/>
-      <c r="M16" s="66"/>
+      <c r="K16" s="83"/>
+      <c r="L16" s="84"/>
+      <c r="M16" s="99"/>
       <c r="N16" s="42"/>
-      <c r="O16" s="64"/>
-      <c r="P16" s="65"/>
-      <c r="Q16" s="66"/>
-      <c r="R16" s="64"/>
-      <c r="S16" s="65"/>
-      <c r="T16" s="66"/>
-      <c r="U16" s="64"/>
-      <c r="V16" s="65"/>
-      <c r="W16" s="66"/>
+      <c r="O16" s="83"/>
+      <c r="P16" s="84"/>
+      <c r="Q16" s="99"/>
+      <c r="R16" s="83"/>
+      <c r="S16" s="84"/>
+      <c r="T16" s="99"/>
+      <c r="U16" s="83"/>
+      <c r="V16" s="84"/>
+      <c r="W16" s="99"/>
     </row>
     <row r="17" spans="2:23" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
@@ -20471,23 +20471,23 @@
       <c r="D17" s="52"/>
       <c r="E17" s="52"/>
       <c r="F17" s="53"/>
-      <c r="G17" s="85"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="87"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="104"/>
+      <c r="I17" s="105"/>
       <c r="J17" s="51"/>
-      <c r="K17" s="85"/>
-      <c r="L17" s="86"/>
-      <c r="M17" s="87"/>
+      <c r="K17" s="103"/>
+      <c r="L17" s="104"/>
+      <c r="M17" s="105"/>
       <c r="N17" s="51"/>
-      <c r="O17" s="85"/>
-      <c r="P17" s="86"/>
-      <c r="Q17" s="87"/>
-      <c r="R17" s="64"/>
-      <c r="S17" s="65"/>
-      <c r="T17" s="66"/>
-      <c r="U17" s="64"/>
-      <c r="V17" s="65"/>
-      <c r="W17" s="66"/>
+      <c r="O17" s="103"/>
+      <c r="P17" s="104"/>
+      <c r="Q17" s="105"/>
+      <c r="R17" s="83"/>
+      <c r="S17" s="84"/>
+      <c r="T17" s="99"/>
+      <c r="U17" s="83"/>
+      <c r="V17" s="84"/>
+      <c r="W17" s="99"/>
     </row>
     <row r="18" spans="2:23" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R18" s="23"/>
@@ -20514,17 +20514,17 @@
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="12"/>
-      <c r="G20" s="76"/>
-      <c r="H20" s="77"/>
-      <c r="I20" s="78"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="91"/>
       <c r="J20" s="46"/>
-      <c r="K20" s="76"/>
-      <c r="L20" s="77"/>
-      <c r="M20" s="78"/>
+      <c r="K20" s="89"/>
+      <c r="L20" s="90"/>
+      <c r="M20" s="91"/>
       <c r="N20" s="46"/>
-      <c r="O20" s="76"/>
-      <c r="P20" s="77"/>
-      <c r="Q20" s="78"/>
+      <c r="O20" s="89"/>
+      <c r="P20" s="90"/>
+      <c r="Q20" s="91"/>
     </row>
     <row r="21" spans="2:23" s="24" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
@@ -20538,13 +20538,13 @@
       <c r="H21" s="48"/>
       <c r="I21" s="49"/>
       <c r="J21" s="48"/>
-      <c r="K21" s="79"/>
-      <c r="L21" s="80"/>
-      <c r="M21" s="80"/>
-      <c r="N21" s="80"/>
-      <c r="O21" s="80"/>
-      <c r="P21" s="80"/>
-      <c r="Q21" s="81"/>
+      <c r="K21" s="94"/>
+      <c r="L21" s="95"/>
+      <c r="M21" s="95"/>
+      <c r="N21" s="95"/>
+      <c r="O21" s="95"/>
+      <c r="P21" s="95"/>
+      <c r="Q21" s="96"/>
     </row>
     <row r="22" spans="2:23" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
@@ -20554,17 +20554,17 @@
       <c r="D22" s="52"/>
       <c r="E22" s="52"/>
       <c r="F22" s="53"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="66"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="99"/>
       <c r="J22" s="42"/>
-      <c r="K22" s="64"/>
-      <c r="L22" s="65"/>
-      <c r="M22" s="66"/>
+      <c r="K22" s="83"/>
+      <c r="L22" s="84"/>
+      <c r="M22" s="99"/>
       <c r="N22" s="42"/>
-      <c r="O22" s="64"/>
-      <c r="P22" s="65"/>
-      <c r="Q22" s="66"/>
+      <c r="O22" s="83"/>
+      <c r="P22" s="84"/>
+      <c r="Q22" s="99"/>
     </row>
     <row r="23" spans="2:23" s="23" customFormat="1" ht="55.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
@@ -20574,17 +20574,17 @@
       <c r="D23" s="52"/>
       <c r="E23" s="52"/>
       <c r="F23" s="53"/>
-      <c r="G23" s="82"/>
-      <c r="H23" s="83"/>
-      <c r="I23" s="84"/>
+      <c r="G23" s="100"/>
+      <c r="H23" s="101"/>
+      <c r="I23" s="102"/>
       <c r="J23" s="50"/>
-      <c r="K23" s="82"/>
-      <c r="L23" s="83"/>
-      <c r="M23" s="84"/>
+      <c r="K23" s="100"/>
+      <c r="L23" s="101"/>
+      <c r="M23" s="102"/>
       <c r="N23" s="50"/>
-      <c r="O23" s="82"/>
-      <c r="P23" s="83"/>
-      <c r="Q23" s="84"/>
+      <c r="O23" s="100"/>
+      <c r="P23" s="101"/>
+      <c r="Q23" s="102"/>
     </row>
     <row r="24" spans="2:23" ht="99.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
@@ -20594,17 +20594,17 @@
       <c r="D24" s="52"/>
       <c r="E24" s="52"/>
       <c r="F24" s="53"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="66"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="84"/>
+      <c r="I24" s="99"/>
       <c r="J24" s="42"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="66"/>
+      <c r="K24" s="83"/>
+      <c r="L24" s="84"/>
+      <c r="M24" s="99"/>
       <c r="N24" s="42"/>
-      <c r="O24" s="64"/>
-      <c r="P24" s="65"/>
-      <c r="Q24" s="66"/>
+      <c r="O24" s="83"/>
+      <c r="P24" s="84"/>
+      <c r="Q24" s="99"/>
     </row>
     <row r="25" spans="2:23" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
@@ -20614,17 +20614,17 @@
       <c r="D25" s="52"/>
       <c r="E25" s="52"/>
       <c r="F25" s="53"/>
-      <c r="G25" s="85"/>
-      <c r="H25" s="86"/>
-      <c r="I25" s="87"/>
+      <c r="G25" s="103"/>
+      <c r="H25" s="104"/>
+      <c r="I25" s="105"/>
       <c r="J25" s="51"/>
-      <c r="K25" s="85"/>
-      <c r="L25" s="86"/>
-      <c r="M25" s="87"/>
+      <c r="K25" s="103"/>
+      <c r="L25" s="104"/>
+      <c r="M25" s="105"/>
       <c r="N25" s="51"/>
-      <c r="O25" s="85"/>
-      <c r="P25" s="86"/>
-      <c r="Q25" s="87"/>
+      <c r="O25" s="103"/>
+      <c r="P25" s="104"/>
+      <c r="Q25" s="105"/>
     </row>
     <row r="26" spans="2:23" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:23" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20636,26 +20636,26 @@
     </row>
     <row r="32" spans="2:23" s="29" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="25"/>
-      <c r="C32" s="70"/>
-      <c r="D32" s="71"/>
-      <c r="E32" s="72"/>
+      <c r="C32" s="106"/>
+      <c r="D32" s="107"/>
+      <c r="E32" s="108"/>
       <c r="F32" s="26"/>
-      <c r="G32" s="70" t="s">
+      <c r="G32" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="H32" s="71"/>
-      <c r="I32" s="72"/>
+      <c r="H32" s="107"/>
+      <c r="I32" s="108"/>
       <c r="J32" s="44"/>
-      <c r="K32" s="73"/>
-      <c r="L32" s="71"/>
-      <c r="M32" s="72"/>
+      <c r="K32" s="64"/>
+      <c r="L32" s="107"/>
+      <c r="M32" s="108"/>
       <c r="N32" s="44"/>
-      <c r="O32" s="73"/>
-      <c r="P32" s="74"/>
-      <c r="Q32" s="75"/>
-      <c r="R32" s="70"/>
-      <c r="S32" s="71"/>
-      <c r="T32" s="72"/>
+      <c r="O32" s="64"/>
+      <c r="P32" s="109"/>
+      <c r="Q32" s="110"/>
+      <c r="R32" s="106"/>
+      <c r="S32" s="107"/>
+      <c r="T32" s="108"/>
     </row>
     <row r="33" spans="2:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="2:2" ht="18" x14ac:dyDescent="0.25">
@@ -20672,38 +20672,47 @@
     </row>
   </sheetData>
   <mergeCells count="86">
-    <mergeCell ref="C2:T2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="R32:T32"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="O25:Q25"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="O32:Q32"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="O23:Q23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="O24:Q24"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="O20:Q20"/>
+    <mergeCell ref="K21:Q21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="O22:Q22"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="O14:Q14"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="U14:W14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="U15:W15"/>
     <mergeCell ref="U11:W11"/>
     <mergeCell ref="K12:Q12"/>
     <mergeCell ref="R12:T12"/>
@@ -20717,47 +20726,38 @@
     <mergeCell ref="K11:M11"/>
     <mergeCell ref="O11:Q11"/>
     <mergeCell ref="R11:T11"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="O15:Q15"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="U15:W15"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="O14:Q14"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="U14:W14"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="O17:Q17"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="O16:Q16"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="U16:W16"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="O20:Q20"/>
-    <mergeCell ref="K21:Q21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="O22:Q22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="O23:Q23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="O24:Q24"/>
-    <mergeCell ref="R32:T32"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="O25:Q25"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="K32:M32"/>
-    <mergeCell ref="O32:Q32"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="C2:T2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="R4:T4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>